<commit_message>
part 5 and 6
</commit_message>
<xml_diff>
--- a/schedule/PDM_Table_Week13.xlsx
+++ b/schedule/PDM_Table_Week13.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\BuiBui's Space\Learning Material\Degree Y3S1\AI Project Management\AIPM-A4\schedule\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{78B9A461-3A7A-4B52-A0BA-97F18838687D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4C3BE26-F4B9-4EAD-97D3-4DAB941762FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{673DD4A1-C9FB-4D04-BCD7-11040A5DF5D1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{673DD4A1-C9FB-4D04-BCD7-11040A5DF5D1}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Part 5" sheetId="1" r:id="rId1"/>
+    <sheet name="Part 6" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="41">
   <si>
     <t>Activity</t>
   </si>
@@ -93,13 +94,79 @@
   </si>
   <si>
     <t>J</t>
+  </si>
+  <si>
+    <t>## Critical Path (PDM)</t>
+  </si>
+  <si>
+    <t>Confirmed Critical Path: Matches AoA (A → J)</t>
+  </si>
+  <si>
+    <t>Activities with zero slack: All (A, B, C, D, E, F, G, H, I, J)</t>
+  </si>
+  <si>
+    <t>Original Duration</t>
+  </si>
+  <si>
+    <t>Crashed Duration</t>
+  </si>
+  <si>
+    <t>Impact / Trade-off</t>
+  </si>
+  <si>
+    <t>E (Model Training)</t>
+  </si>
+  <si>
+    <t>5 days</t>
+  </si>
+  <si>
+    <t>3 days</t>
+  </si>
+  <si>
+    <t>Trade-off: Increases "Hardware / Cloud" budget (estimated RM100 in Cost Sheet) but mitigates Risk R6 (Limited GPU resources 1).</t>
+  </si>
+  <si>
+    <t>H (Testing &amp; Validation)</t>
+  </si>
+  <si>
+    <t>4 days</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cost/Resource: Reallocate the "QA Tester" (Hor Ying Huai) to work overtime or assign the "Development Team" to assist in parallel testing. </t>
+  </si>
+  <si>
+    <t>Part 6: Schedule Crashing Analysis</t>
+  </si>
+  <si>
+    <t>Part 5: Precedence Diagram Method (PDM)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cost/Resource: Rent high-performance GPUs (e.g., RepoCloud or Colab Pro) to accelerate the training epochs. </t>
+  </si>
+  <si>
+    <t>Trade-off: Reduces team focus on documentation, increases burnout risk (Risk R5 2).</t>
+  </si>
+  <si>
+    <t>Recalculate Schedule:</t>
+  </si>
+  <si>
+    <t>Original Duration: 36 Days</t>
+  </si>
+  <si>
+    <t>Savings: 2 days (Activity E) + 1 day (Activity H) = 3 days saved.</t>
+  </si>
+  <si>
+    <t>New Project Duration: 33 Days</t>
+  </si>
+  <si>
+    <t>Was crashing effective? Yes. It reduced the schedule by 3 days. However, strictly crashing "Model Training" is risky because your team noted that training outcomes are "inherently unpredictable" and often require a buffer rather than a reduction.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -108,6 +175,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -135,17 +218,134 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="16">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -300,17 +500,30 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0F0A01D5-EF2E-499C-A7C9-B8A582E71D76}" name="Table2" displayName="Table2" ref="A1:H11" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
-  <autoFilter ref="A1:H11" xr:uid="{0F0A01D5-EF2E-499C-A7C9-B8A582E71D76}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0F0A01D5-EF2E-499C-A7C9-B8A582E71D76}" name="Table2" displayName="Table2" ref="A2:H12" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A2:H12" xr:uid="{0F0A01D5-EF2E-499C-A7C9-B8A582E71D76}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{5E7E3DA3-A2E5-45DA-A6A0-B0924A5E88BD}" name="Activity" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{7BB9A3BD-37B3-44B8-8F0E-91D8AAEE99D4}" name="Duration" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{065C7403-6B14-4721-A0FB-F0442E101427}" name="Predecessor" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{9DB507F2-3FBA-4265-B8F6-2F6AFA12745D}" name="ES" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{59ACB1F1-BD40-4C8F-A37F-97D3C0F579E5}" name="EF" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{2977EAA5-2AD3-47A9-9E9A-D85F3211F250}" name="LS" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{774EA564-273C-4998-A791-C168E7401D28}" name="LF" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{F87F2C08-F758-47C5-B33E-02C0667C4967}" name="Slack" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{5E7E3DA3-A2E5-45DA-A6A0-B0924A5E88BD}" name="Activity" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{7BB9A3BD-37B3-44B8-8F0E-91D8AAEE99D4}" name="Duration" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{065C7403-6B14-4721-A0FB-F0442E101427}" name="Predecessor" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{9DB507F2-3FBA-4265-B8F6-2F6AFA12745D}" name="ES" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{59ACB1F1-BD40-4C8F-A37F-97D3C0F579E5}" name="EF" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{2977EAA5-2AD3-47A9-9E9A-D85F3211F250}" name="LS" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{774EA564-273C-4998-A791-C168E7401D28}" name="LF" dataDxfId="9"/>
+    <tableColumn id="8" xr3:uid="{F87F2C08-F758-47C5-B33E-02C0667C4967}" name="Slack" dataDxfId="8"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{37F1AB9A-338F-464F-853A-DF8493270666}" name="Table4" displayName="Table4" ref="A2:D6" totalsRowShown="0" headerRowDxfId="4" dataDxfId="5">
+  <autoFilter ref="A2:D6" xr:uid="{37F1AB9A-338F-464F-853A-DF8493270666}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{C7711C89-F05B-46B4-AB7C-A458FD8C7322}" name="Activity" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{E9A1DD50-66A9-4490-8501-442731DAB3EF}" name="Original Duration" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{4011381F-8BA2-4CE7-BD28-DB83928924DA}" name="Crashed Duration" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{C9ACC6FD-7759-40AB-9CAE-D362EB51B93E}" name="Impact / Trade-off" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -633,10 +846,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD49B865-4708-401D-88C5-1C409B8F089F}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:Q25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -648,78 +861,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="2">
-        <v>3</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="2">
-        <v>0</v>
-      </c>
-      <c r="E2" s="2">
-        <v>3</v>
-      </c>
-      <c r="F2" s="2">
-        <v>0</v>
-      </c>
-      <c r="G2" s="2">
-        <v>3</v>
-      </c>
-      <c r="H2" s="2">
-        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B3" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D3" s="2">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2">
         <v>3</v>
       </c>
-      <c r="E3" s="2">
-        <v>7</v>
-      </c>
       <c r="F3" s="2">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2">
         <v>3</v>
-      </c>
-      <c r="G3" s="2">
-        <v>7</v>
       </c>
       <c r="H3" s="2">
         <v>0</v>
@@ -727,25 +919,25 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="2">
         <v>4</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D4" s="2">
+        <v>3</v>
+      </c>
+      <c r="E4" s="2">
         <v>7</v>
       </c>
-      <c r="E4" s="2">
-        <v>11</v>
-      </c>
       <c r="F4" s="2">
+        <v>3</v>
+      </c>
+      <c r="G4" s="2">
         <v>7</v>
-      </c>
-      <c r="G4" s="2">
-        <v>11</v>
       </c>
       <c r="H4" s="2">
         <v>0</v>
@@ -753,25 +945,25 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" s="2">
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="2">
+        <v>7</v>
+      </c>
+      <c r="E5" s="2">
         <v>11</v>
       </c>
-      <c r="D5" s="2">
+      <c r="F5" s="2">
+        <v>7</v>
+      </c>
+      <c r="G5" s="2">
         <v>11</v>
-      </c>
-      <c r="E5" s="2">
-        <v>15</v>
-      </c>
-      <c r="F5" s="2">
-        <v>11</v>
-      </c>
-      <c r="G5" s="2">
-        <v>15</v>
       </c>
       <c r="H5" s="2">
         <v>0</v>
@@ -779,25 +971,25 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D6" s="2">
+        <v>11</v>
+      </c>
+      <c r="E6" s="2">
         <v>15</v>
       </c>
-      <c r="E6" s="2">
-        <v>20</v>
-      </c>
       <c r="F6" s="2">
+        <v>11</v>
+      </c>
+      <c r="G6" s="2">
         <v>15</v>
-      </c>
-      <c r="G6" s="2">
-        <v>20</v>
       </c>
       <c r="H6" s="2">
         <v>0</v>
@@ -805,25 +997,25 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D7" s="2">
+        <v>15</v>
+      </c>
+      <c r="E7" s="2">
         <v>20</v>
       </c>
-      <c r="E7" s="2">
-        <v>24</v>
-      </c>
       <c r="F7" s="2">
+        <v>15</v>
+      </c>
+      <c r="G7" s="2">
         <v>20</v>
-      </c>
-      <c r="G7" s="2">
-        <v>24</v>
       </c>
       <c r="H7" s="2">
         <v>0</v>
@@ -831,25 +1023,25 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" s="2">
         <v>4</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D8" s="2">
+        <v>20</v>
+      </c>
+      <c r="E8" s="2">
         <v>24</v>
       </c>
-      <c r="E8" s="2">
-        <v>28</v>
-      </c>
       <c r="F8" s="2">
+        <v>20</v>
+      </c>
+      <c r="G8" s="2">
         <v>24</v>
-      </c>
-      <c r="G8" s="2">
-        <v>28</v>
       </c>
       <c r="H8" s="2">
         <v>0</v>
@@ -857,25 +1049,25 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" s="2">
         <v>4</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D9" s="2">
+        <v>24</v>
+      </c>
+      <c r="E9" s="2">
         <v>28</v>
       </c>
-      <c r="E9" s="2">
-        <v>32</v>
-      </c>
       <c r="F9" s="2">
+        <v>24</v>
+      </c>
+      <c r="G9" s="2">
         <v>28</v>
-      </c>
-      <c r="G9" s="2">
-        <v>32</v>
       </c>
       <c r="H9" s="2">
         <v>0</v>
@@ -883,25 +1075,25 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B10" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D10" s="2">
+        <v>28</v>
+      </c>
+      <c r="E10" s="2">
         <v>32</v>
       </c>
-      <c r="E10" s="2">
-        <v>35</v>
-      </c>
       <c r="F10" s="2">
+        <v>28</v>
+      </c>
+      <c r="G10" s="2">
         <v>32</v>
-      </c>
-      <c r="G10" s="2">
-        <v>35</v>
       </c>
       <c r="H10" s="2">
         <v>0</v>
@@ -909,28 +1101,272 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D11" s="2">
+        <v>32</v>
+      </c>
+      <c r="E11" s="2">
         <v>35</v>
       </c>
-      <c r="E11" s="2">
-        <v>36</v>
-      </c>
       <c r="F11" s="2">
+        <v>32</v>
+      </c>
+      <c r="G11" s="2">
         <v>35</v>
-      </c>
-      <c r="G11" s="2">
-        <v>36</v>
       </c>
       <c r="H11" s="2">
         <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="2">
+        <v>1</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="2">
+        <v>35</v>
+      </c>
+      <c r="E12" s="2">
+        <v>36</v>
+      </c>
+      <c r="F12" s="2">
+        <v>35</v>
+      </c>
+      <c r="G12" s="2">
+        <v>36</v>
+      </c>
+      <c r="H12" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A16:H16"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B65D8C58-73B1-4D4B-A744-1138DFA26799}">
+  <dimension ref="A1:Q12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="33.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.77734375" customWidth="1"/>
+    <col min="3" max="3" width="18.5546875" customWidth="1"/>
+    <col min="4" max="4" width="126.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+    </row>
+    <row r="2" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+    </row>
+    <row r="3" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+    </row>
+    <row r="4" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+    </row>
+    <row r="5" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+    </row>
+    <row r="6" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>